<commit_message>
trying to resolve timing issue
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0C840E-2CCF-4104-9F8E-13A8D5290100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A49255-07A9-4243-9115-440BD933C325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -77,6 +77,41 @@
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
   <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
+ WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(f.file_type, '') AS `File Type`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `File Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
 WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
@@ -93,43 +128,7 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
- WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
   </si>
 </sst>
 </file>
@@ -501,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,12 +529,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -552,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>
@@ -569,7 +568,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
updated ubc2 10 scripts, renamed test suites with w, commiting stashed changes
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A49255-07A9-4243-9115-440BD933C325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D8878C-168D-4893-8567-369183805DB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -504,15 +504,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -546,7 +546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -563,7 +563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -580,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ccdc curated suite and data
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\May\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D8878C-168D-4893-8567-369183805DB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516719E9-22F3-40C8-8AD5-0305B4E1B25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -61,20 +61,6 @@
   </si>
   <si>
     <t>TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)
-  MATCH (demo:demographic) 
-  MATCH (diag:diagnosis)
- MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-	WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
-OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case)
-OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)&lt;-[:of_sample]-(f:file)
-RETURN 
-	count(DISTINCT(f)) as number_of_files , 
-	count(DISTINCT(samp)) as number_of_sample , 
-	count(DISTINCT(c.case_id)) as number_of_cases , 
-	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
@@ -112,23 +98,74 @@
         coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 MATCH (c)&lt;--(diag:diagnosis)
+MATCH (f:file)-[*]-&gt;(samp:sample)--&gt;(c)
+MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp,demo, c, s, p, diag
 WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
+RETURN
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+MATCH (sf:file)--&gt;(s)
+MATCH (s)&lt;--(c)
+MATCH (samp:sample)--&gt;(c)
+WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
+WITH DISTINCT f,  s, c
+WITH
+        f, c,  s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c,  s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c,   s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis) 
+ MATCH (samp:sample)--&gt;(c)
+WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
 OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+       coalesce(c.case_id, '') AS `Case ID`,
+       coalesce(s.clinical_study_designation, '') AS `Study Code`,
+       coalesce(s.clinical_study_type, '') AS  `Study Type`,
+       coalesce(demo.breed, '') AS Breed ,
+       coalesce(diag.disease_term, '') AS Diagnosis ,
+       coalesce(diag.stage_of_disease, '') AS `Stage of Disease`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+       coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+Order by c.case_id LIMIT 100        </t>
   </si>
 </sst>
 </file>
@@ -500,19 +537,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.81640625" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -529,15 +566,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -546,15 +583,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -563,15 +600,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -580,7 +617,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ICDC UBC02 changes and MTP 22.11 3 tickets update
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
+++ b/InputFiles/TC01_Canine_StudyUBC02-Breed_Diagnosis_PrimDiseaseSite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\May\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516719E9-22F3-40C8-8AD5-0305B4E1B25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D035C21-1799-4141-ABA8-6917EF4F5CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -78,24 +78,6 @@
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
   <si>
     <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -166,6 +148,40 @@
        coalesce(diag.best_response, '') AS `Response to Treatment`,
        coalesce(co.cohort_description, '') AS `Cohort`
 Order by c.case_id LIMIT 100        </t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['UBC02'] and demo.breed in ['Beagle','Mixed Breed']and diag.disease_term in ['Bladder Cancer','Healthy Control'] and diag.primary_disease_site in ['Bladder, Urethra']
+WITH DISTINCT f, parent, c, demo, diag, s
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+ coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`, 
+      CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+   coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis 
+        Order By f.file_name LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -537,19 +553,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="77.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -566,15 +582,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -583,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -591,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -600,15 +616,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -617,15 +633,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -634,7 +650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>